<commit_message>
version one of vlookup page and tile are live
</commit_message>
<xml_diff>
--- a/assets/excel file/Product Catalog Database for VLOOKUP and Advanced Filters.xlsx
+++ b/assets/excel file/Product Catalog Database for VLOOKUP and Advanced Filters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hao\Desktop\Hao Dong io\haodong191.github.io\assets\excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F179D025-5F46-41B8-AB9E-CDB0CDCE8863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E8EF33-9C31-4052-8AA1-04D0AF51D0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{3DA30817-AB17-418F-A166-367311C102B0}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1525,7 +1525,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1538,10 +1538,10 @@
     <xf numFmtId="44" fontId="19" fillId="33" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="18" fillId="34" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="19" fillId="34" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1551,7 +1551,6 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1931,7 +1930,7 @@
   <dimension ref="A1:R98"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5310,10 +5309,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5757CD10-E47D-4E0D-88D7-4BA8D2B4C350}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S102"/>
+  <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5333,39 +5332,39 @@
     <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>18</v>
       </c>
@@ -5373,10 +5372,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L4" s="11"/>
-    </row>
-    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -5410,7 +5406,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -5441,16 +5437,11 @@
       <c r="J6">
         <v>4</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -5481,14 +5472,9 @@
       <c r="J7">
         <v>4</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5519,13 +5505,8 @@
       <c r="J8">
         <v>2</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-    </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -5557,7 +5538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -5588,9 +5569,9 @@
       <c r="J10">
         <v>2</v>
       </c>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -5622,7 +5603,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -5654,7 +5635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -5686,7 +5667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -5718,7 +5699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -5750,7 +5731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -6294,7 +6275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -6326,7 +6307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -6358,7 +6339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -6390,7 +6371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -6422,7 +6403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -6454,7 +6435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>116</v>
       </c>
@@ -6485,12 +6466,8 @@
       <c r="J38">
         <v>10</v>
       </c>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-    </row>
-    <row r="39" spans="1:19" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:18" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -6524,9 +6501,8 @@
       <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
-      <c r="S39" s="11"/>
-    </row>
-    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -6557,12 +6533,8 @@
       <c r="J40">
         <v>2</v>
       </c>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-    </row>
-    <row r="41" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -6593,12 +6565,8 @@
       <c r="J41">
         <v>8</v>
       </c>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-    </row>
-    <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -6629,12 +6597,8 @@
       <c r="J42">
         <v>3</v>
       </c>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-    </row>
-    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>130</v>
       </c>
@@ -6665,12 +6629,8 @@
       <c r="J43">
         <v>10</v>
       </c>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="11"/>
-    </row>
-    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>134</v>
       </c>
@@ -6701,12 +6661,8 @@
       <c r="J44">
         <v>1</v>
       </c>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
-    </row>
-    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -6738,7 +6694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>138</v>
       </c>
@@ -6770,7 +6726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -6802,7 +6758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>142</v>
       </c>
@@ -8572,7 +8528,7 @@
   <dimension ref="A2:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8590,7 +8546,7 @@
     <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -8600,10 +8556,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="13" t="s">
         <v>289</v>
       </c>
       <c r="N2" s="3" t="s">
@@ -8641,34 +8597,34 @@
       <c r="J5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="U5" s="11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>